<commit_message>
Version: 0.0.16. Bug fixes
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -7,17 +7,19 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Example Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Example Sheet 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Example Sheet 1'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Example Sheet 2'!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Column 1</t>
   </si>
@@ -440,4 +442,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625"/>
+    <col min="3" max="3" width="9.140625"/>
+    <col min="4" max="4" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>